<commit_message>
updated metadata in results
</commit_message>
<xml_diff>
--- a/src/openai_client/2026-02-09-20-37-15-llm_direct_answer_results_gpt5_mini_reasoning_high.xlsx
+++ b/src/openai_client/2026-02-09-20-37-15-llm_direct_answer_results_gpt5_mini_reasoning_high.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ralf\PycharmProjects\llms-for-math\src\openai_client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1A16D6-3F85-48AC-970F-C53A84A75369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ED6B93-FA5E-4340-9451-211E6D341031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33017" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33017" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Answer data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4088" uniqueCount="1200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4090" uniqueCount="1202">
   <si>
     <t>row_idx</t>
   </si>
@@ -4548,6 +4548,12 @@
   </si>
   <si>
     <t>Better use verbosity = medium.</t>
+  </si>
+  <si>
+    <t>(reasonable cost even with reasoning tokens)</t>
+  </si>
+  <si>
+    <t>max output tokens = 10.000 (default) - rarely used with verbosity low</t>
   </si>
 </sst>
 </file>
@@ -52629,10 +52635,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1CD584-23AD-422F-A125-95727BAFE535}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -52660,21 +52666,29 @@
       <c r="B3" t="s">
         <v>1171</v>
       </c>
+      <c r="D3" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1173</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>1172</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
         <v>1182</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C5" t="s">
         <v>1183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>1201</v>
       </c>
     </row>
   </sheetData>
@@ -52686,7 +52700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41E9D33-B80B-4FB3-9D41-A9302311E82B}">
   <dimension ref="A3:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated LLM direct answer results with wrap-up
</commit_message>
<xml_diff>
--- a/src/openai_client/2026-02-09-20-37-15-llm_direct_answer_results_gpt5_mini_reasoning_high.xlsx
+++ b/src/openai_client/2026-02-09-20-37-15-llm_direct_answer_results_gpt5_mini_reasoning_high.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ralf\PycharmProjects\llms-for-math\src\openai_client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ED6B93-FA5E-4340-9451-211E6D341031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F2A882-32D4-4B05-87AF-292BCD8CE375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33017" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24171" yWindow="951" windowWidth="24685" windowHeight="13055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Answer data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -16350,7 +16350,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13684B5C-EA28-4964-A0C8-DF4F6788F989}" name="PivotTable1" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{13684B5C-EA28-4964-A0C8-DF4F6788F989}" name="PivotTable1" cacheId="2" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:M13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
@@ -16485,7 +16485,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F52D719B-098E-4391-8E13-386D01B68AB8}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F52D719B-098E-4391-8E13-386D01B68AB8}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C140" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField axis="axisRow" showAll="0">
@@ -52637,8 +52637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1CD584-23AD-422F-A125-95727BAFE535}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -52700,8 +52700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41E9D33-B80B-4FB3-9D41-A9302311E82B}">
   <dimension ref="A3:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -53179,8 +53179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04E7BB9-82BA-43B3-B835-24C96FE3F124}">
   <dimension ref="A3:C140"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>